<commit_message>
Language fixes (still incomplete)
</commit_message>
<xml_diff>
--- a/docassemble/MAEvictionDefense/data/sources/eviction_vi.xlsx
+++ b/docassemble/MAEvictionDefense/data/sources/eviction_vi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QSteenhuis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QSteenhuis\Google Drive\eviction-interview\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11940"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26207,7 +26207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26239,6 +26239,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -26260,7 +26267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -26277,6 +26284,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -26586,8 +26597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="H187" sqref="H187"/>
+    <sheetView tabSelected="1" topLeftCell="G496" workbookViewId="0">
+      <selection activeCell="H338" sqref="H338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38350,7 +38361,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A453" s="2" t="s">
         <v>291</v>
       </c>
@@ -38372,11 +38383,11 @@
       <c r="G453" s="3" t="s">
         <v>1391</v>
       </c>
-      <c r="H453" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H453" s="7" t="s">
+        <v>2191</v>
+      </c>
+    </row>
+    <row r="454" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A454" s="2" t="s">
         <v>291</v>
       </c>
@@ -38398,11 +38409,11 @@
       <c r="G454" s="3" t="s">
         <v>1393</v>
       </c>
-      <c r="H454" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H454" s="7" t="s">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="455" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A455" s="2" t="s">
         <v>291</v>
       </c>
@@ -38424,11 +38435,11 @@
       <c r="G455" s="3" t="s">
         <v>1395</v>
       </c>
-      <c r="H455" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H455" s="7" t="s">
+        <v>2176</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A456" s="2" t="s">
         <v>291</v>
       </c>
@@ -38450,11 +38461,11 @@
       <c r="G456" s="3" t="s">
         <v>1397</v>
       </c>
-      <c r="H456" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H456" s="7" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A457" s="2" t="s">
         <v>291</v>
       </c>
@@ -38476,11 +38487,11 @@
       <c r="G457" s="3" t="s">
         <v>1399</v>
       </c>
-      <c r="H457" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H457" s="7" t="s">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A458" s="2" t="s">
         <v>291</v>
       </c>
@@ -38502,11 +38513,11 @@
       <c r="G458" s="3" t="s">
         <v>1401</v>
       </c>
-      <c r="H458" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H458" s="7" t="s">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A459" s="2" t="s">
         <v>291</v>
       </c>
@@ -38528,11 +38539,11 @@
       <c r="G459" s="3" t="s">
         <v>1403</v>
       </c>
-      <c r="H459" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H459" s="7" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A460" s="2" t="s">
         <v>291</v>
       </c>
@@ -38554,11 +38565,11 @@
       <c r="G460" s="3" t="s">
         <v>1405</v>
       </c>
-      <c r="H460" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H460" s="7" t="s">
+        <v>2182</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A461" s="2" t="s">
         <v>291</v>
       </c>
@@ -38580,11 +38591,11 @@
       <c r="G461" s="3" t="s">
         <v>1407</v>
       </c>
-      <c r="H461" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H461" s="7" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A462" s="2" t="s">
         <v>291</v>
       </c>
@@ -38606,11 +38617,11 @@
       <c r="G462" s="3" t="s">
         <v>1409</v>
       </c>
-      <c r="H462" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H462" s="7" t="s">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="463" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A463" s="2" t="s">
         <v>291</v>
       </c>
@@ -38632,11 +38643,11 @@
       <c r="G463" s="3" t="s">
         <v>1411</v>
       </c>
-      <c r="H463" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H463" s="7" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A464" s="2" t="s">
         <v>291</v>
       </c>
@@ -38658,11 +38669,11 @@
       <c r="G464" s="3" t="s">
         <v>1413</v>
       </c>
-      <c r="H464" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H464" s="7" t="s">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="465" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A465" s="2" t="s">
         <v>291</v>
       </c>
@@ -38684,11 +38695,11 @@
       <c r="G465" s="3" t="s">
         <v>1415</v>
       </c>
-      <c r="H465" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H465" s="7" t="s">
+        <v>2226</v>
+      </c>
+    </row>
+    <row r="466" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A466" s="2" t="s">
         <v>291</v>
       </c>
@@ -38710,8 +38721,8 @@
       <c r="G466" s="3" t="s">
         <v>1417</v>
       </c>
-      <c r="H466" s="4" t="s">
-        <v>369</v>
+      <c r="H466" s="7" t="s">
+        <v>2209</v>
       </c>
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>